<commit_message>
- DS khách hang: add some column {thu/chi khachHang, tong gtri sudung}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>DANH SÁCH KHÁCH HÀNG</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>Số tài khoản</t>
+  </si>
+  <si>
+    <t>Tổng gtrị thanh toán</t>
+  </si>
+  <si>
+    <t>Tổng hoàn cọc</t>
+  </si>
+  <si>
+    <t>Tổng gtrị sử dụng</t>
+  </si>
+  <si>
+    <t>Tổng hoàn dịch vụ</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
   </si>
 </sst>
 </file>
@@ -139,7 +154,7 @@
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +166,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,12 +196,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,34 +335,37 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -621,11 +671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,44 +692,48 @@
     <col min="11" max="16" width="24.140625" style="14" customWidth="1"/>
     <col min="17" max="17" width="24.140625" style="36" customWidth="1"/>
     <col min="18" max="19" width="18" style="9" customWidth="1"/>
-    <col min="20" max="20" width="26.140625" style="9" customWidth="1"/>
-    <col min="21" max="21" width="20" style="32" customWidth="1"/>
-    <col min="22" max="22" width="24.5703125" style="21" customWidth="1"/>
-    <col min="23" max="23" width="27.7109375" style="28" customWidth="1"/>
-    <col min="24" max="24" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="24" width="26.140625" style="9" customWidth="1"/>
+    <col min="25" max="25" width="20" style="32" customWidth="1"/>
+    <col min="26" max="26" width="24.5703125" style="21" customWidth="1"/>
+    <col min="27" max="27" width="27.7109375" style="28" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="6"/>
-    </row>
-    <row r="3" spans="1:25" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="6"/>
+    </row>
+    <row r="3" spans="1:29" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -740,20 +794,32 @@
       <c r="T3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="U3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="Z3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="AA3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="AB3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="11"/>
       <c r="C4" s="7"/>
@@ -774,12 +840,16 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
@@ -800,12 +870,16 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="7"/>
@@ -826,12 +900,16 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="7"/>
@@ -852,12 +930,16 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="11"/>
       <c r="C8" s="7"/>
@@ -878,12 +960,16 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="11"/>
       <c r="C9" s="7"/>
@@ -904,12 +990,16 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
@@ -930,12 +1020,16 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="11"/>
       <c r="C11" s="7"/>
@@ -956,12 +1050,16 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
@@ -982,12 +1080,16 @@
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
@@ -1008,12 +1110,16 @@
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -1034,12 +1140,16 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -1060,12 +1170,16 @@
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -1086,12 +1200,16 @@
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="26"/>
+      <c r="AB16" s="26"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -1112,12 +1230,16 @@
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -1138,12 +1260,16 @@
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
@@ -1164,12 +1290,16 @@
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
@@ -1190,12 +1320,16 @@
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
@@ -1216,12 +1350,16 @@
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
@@ -1242,12 +1380,16 @@
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
@@ -1268,12 +1410,16 @@
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
@@ -1294,12 +1440,16 @@
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -1320,12 +1470,16 @@
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="26"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1346,78 +1500,135 @@
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
-    </row>
-    <row r="27" spans="1:24" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="39">
-        <f>SUM(R4:R26)</f>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="26"/>
+    </row>
+    <row r="28" spans="1:28" s="47" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="40">
+        <f>SUM(R$4:R26)</f>
         <v>0</v>
       </c>
-      <c r="S27" s="39">
-        <f>SUM(S4:S26)</f>
+      <c r="S28" s="40">
+        <f>SUM(S$4:S26)</f>
         <v>0</v>
       </c>
-      <c r="T27" s="39">
-        <f>SUM(T4:T26)</f>
+      <c r="T28" s="40">
+        <f>SUM(T$4:T26)</f>
         <v>0</v>
       </c>
-      <c r="U27" s="39">
-        <f>SUM(U4:U26)</f>
+      <c r="U28" s="40">
+        <f>SUM(U$4:U26)</f>
         <v>0</v>
       </c>
-      <c r="V27" s="42"/>
-      <c r="W27" s="44"/>
-      <c r="X27" s="44"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
+      <c r="V28" s="40">
+        <f>SUM(V$4:V26)</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="40">
+        <f>SUM(W$4:W26)</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="40">
+        <f>SUM(X$4:X26)</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="40">
+        <f>SUM(Y$4:Y26)</f>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="43"/>
+      <c r="AA28" s="46"/>
+      <c r="AB28" s="46"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="24"/>
+      <c r="AA29" s="27"/>
+      <c r="AB29" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:X1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
DS KhachHang: remove some column
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DANH SÁCH KHÁCH HÀNG</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Ngày sinh</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Địa chỉ</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Tổng bán</t>
   </si>
   <si>
-    <t>Tổng bán trừ trả hàng</t>
-  </si>
-  <si>
     <t>Nguồn khách</t>
   </si>
   <si>
@@ -64,21 +58,9 @@
     <t>Người tạo</t>
   </si>
   <si>
-    <t>Tổng tích điểm</t>
-  </si>
-  <si>
-    <t>Trạng thái khách hàng</t>
-  </si>
-  <si>
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>Ngày giao dịch gần nhất</t>
-  </si>
-  <si>
-    <t>Mã số thuế</t>
-  </si>
-  <si>
     <t>Tỉnh thành</t>
   </si>
   <si>
@@ -89,9 +71,6 @@
   </si>
   <si>
     <t>Ngày tạo</t>
-  </si>
-  <si>
-    <t>Số tài khoản</t>
   </si>
   <si>
     <t>Tổng gtrị thanh toán</t>
@@ -227,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -311,18 +290,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -335,6 +302,25 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,28 +330,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -671,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,54 +650,42 @@
     <col min="4" max="4" width="22.85546875" style="14" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="18" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="10" customWidth="1"/>
-    <col min="8" max="9" width="23.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="34.85546875" style="25" customWidth="1"/>
-    <col min="11" max="16" width="24.140625" style="14" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" style="36" customWidth="1"/>
-    <col min="18" max="19" width="18" style="9" customWidth="1"/>
-    <col min="20" max="24" width="26.140625" style="9" customWidth="1"/>
-    <col min="25" max="25" width="20" style="32" customWidth="1"/>
-    <col min="26" max="26" width="24.5703125" style="21" customWidth="1"/>
-    <col min="27" max="27" width="27.7109375" style="28" customWidth="1"/>
-    <col min="28" max="28" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="34.85546875" style="25" customWidth="1"/>
+    <col min="8" max="13" width="24.140625" style="14" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="32" customWidth="1"/>
+    <col min="15" max="15" width="18" style="9" customWidth="1"/>
+    <col min="16" max="20" width="26.140625" style="9" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="6"/>
-    </row>
-    <row r="3" spans="1:29" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="6"/>
+    </row>
+    <row r="3" spans="1:22" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -752,882 +704,673 @@
       <c r="F3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
+      <c r="H3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="11"/>
       <c r="C4" s="7"/>
       <c r="D4" s="16"/>
       <c r="E4" s="19"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
       <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="34"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U4" s="26"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
       <c r="D5" s="16"/>
       <c r="E5" s="19"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
       <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="34"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U5" s="26"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="7"/>
       <c r="D6" s="16"/>
       <c r="E6" s="19"/>
       <c r="F6" s="23"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
       <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="34"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U6" s="26"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="7"/>
       <c r="D7" s="16"/>
       <c r="E7" s="19"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="34"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U7" s="26"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="11"/>
       <c r="C8" s="7"/>
       <c r="D8" s="16"/>
       <c r="E8" s="19"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="34"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U8" s="26"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="11"/>
       <c r="C9" s="7"/>
       <c r="D9" s="16"/>
       <c r="E9" s="19"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="34"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U9" s="26"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="34"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U10" s="26"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="34"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U11" s="26"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="34"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U12" s="26"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="34"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="26"/>
-      <c r="AB13" s="26"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U13" s="26"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
       <c r="D14" s="16"/>
       <c r="E14" s="19"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="34"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U14" s="26"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
       <c r="D15" s="16"/>
       <c r="E15" s="19"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="34"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U15" s="26"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
       <c r="D16" s="16"/>
       <c r="E16" s="19"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="34"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U16" s="26"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
       <c r="D17" s="16"/>
       <c r="E17" s="19"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="34"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U17" s="26"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
       <c r="D18" s="16"/>
       <c r="E18" s="19"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="34"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U18" s="26"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
       <c r="D19" s="16"/>
       <c r="E19" s="19"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="34"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="30"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U19" s="26"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
       <c r="D20" s="16"/>
       <c r="E20" s="19"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="34"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U20" s="26"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
       <c r="D21" s="16"/>
       <c r="E21" s="19"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="34"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U21" s="26"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
       <c r="D22" s="16"/>
       <c r="E22" s="19"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="34"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U22" s="26"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
       <c r="D23" s="16"/>
       <c r="E23" s="19"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="34"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="30"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U23" s="26"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
       <c r="D24" s="16"/>
       <c r="E24" s="19"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="34"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="23"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U24" s="26"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
       <c r="D25" s="16"/>
       <c r="E25" s="19"/>
       <c r="F25" s="23"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="34"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="23"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U25" s="26"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
       <c r="D26" s="16"/>
       <c r="E26" s="19"/>
       <c r="F26" s="23"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="34"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="23"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U26" s="26"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
       <c r="D27" s="16"/>
       <c r="E27" s="19"/>
       <c r="F27" s="23"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="34"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="26"/>
-    </row>
-    <row r="28" spans="1:28" s="47" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="40">
+      <c r="U27" s="26"/>
+    </row>
+    <row r="28" spans="1:21" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="42"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="33">
+        <f>SUM(O$4:O26)</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="33">
+        <f>SUM(P$4:P26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="33">
+        <f>SUM(Q$4:Q26)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="33">
         <f>SUM(R$4:R26)</f>
         <v>0</v>
       </c>
-      <c r="S28" s="40">
+      <c r="S28" s="33">
         <f>SUM(S$4:S26)</f>
         <v>0</v>
       </c>
-      <c r="T28" s="40">
+      <c r="T28" s="33">
         <f>SUM(T$4:T26)</f>
         <v>0</v>
       </c>
-      <c r="U28" s="40">
-        <f>SUM(U$4:U26)</f>
-        <v>0</v>
-      </c>
-      <c r="V28" s="40">
-        <f>SUM(V$4:V26)</f>
-        <v>0</v>
-      </c>
-      <c r="W28" s="40">
-        <f>SUM(W$4:W26)</f>
-        <v>0</v>
-      </c>
-      <c r="X28" s="40">
-        <f>SUM(X$4:X26)</f>
-        <v>0</v>
-      </c>
-      <c r="Y28" s="40">
-        <f>SUM(Y$4:Y26)</f>
-        <v>0</v>
-      </c>
-      <c r="Z28" s="43"/>
-      <c r="AA28" s="46"/>
-      <c r="AB28" s="46"/>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U28" s="38"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="12"/>
       <c r="C29" s="8"/>
       <c r="D29" s="17"/>
       <c r="E29" s="20"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="35"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="31"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
+      <c r="U29" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="A1:U1"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>

<commit_message>
DSKhachHang: add column {SoTienChuaSD}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>DANH SÁCH KHÁCH HÀNG</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Tổng cộng</t>
+  </si>
+  <si>
+    <t>Số tiền chưa sử dụng</t>
   </si>
 </sst>
 </file>
@@ -635,11 +638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,12 +657,12 @@
     <col min="8" max="13" width="24.140625" style="14" customWidth="1"/>
     <col min="14" max="14" width="24.140625" style="32" customWidth="1"/>
     <col min="15" max="15" width="18" style="9" customWidth="1"/>
-    <col min="16" max="20" width="26.140625" style="9" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="21" width="26.140625" style="9" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -683,9 +686,10 @@
       <c r="S1" s="40"/>
       <c r="T1" s="40"/>
       <c r="U1" s="40"/>
-      <c r="V1" s="6"/>
-    </row>
-    <row r="3" spans="1:22" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V1" s="40"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="3" spans="1:23" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -746,11 +750,14 @@
       <c r="T3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="11"/>
       <c r="C4" s="7"/>
@@ -771,9 +778,10 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
-      <c r="U4" s="26"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U4" s="7"/>
+      <c r="V4" s="26"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
@@ -794,9 +802,10 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="26"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U5" s="7"/>
+      <c r="V5" s="26"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="7"/>
@@ -817,9 +826,10 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="26"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U6" s="7"/>
+      <c r="V6" s="26"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="7"/>
@@ -840,9 +850,10 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="26"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U7" s="7"/>
+      <c r="V7" s="26"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="11"/>
       <c r="C8" s="7"/>
@@ -863,9 +874,10 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="26"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U8" s="7"/>
+      <c r="V8" s="26"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="11"/>
       <c r="C9" s="7"/>
@@ -886,9 +898,10 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="26"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+      <c r="V9" s="26"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
@@ -909,9 +922,10 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="26"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U10" s="7"/>
+      <c r="V10" s="26"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="11"/>
       <c r="C11" s="7"/>
@@ -932,9 +946,10 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="26"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U11" s="7"/>
+      <c r="V11" s="26"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
@@ -955,9 +970,10 @@
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
-      <c r="U12" s="26"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U12" s="7"/>
+      <c r="V12" s="26"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
@@ -978,9 +994,10 @@
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
-      <c r="U13" s="26"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U13" s="7"/>
+      <c r="V13" s="26"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -1001,9 +1018,10 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="26"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U14" s="7"/>
+      <c r="V14" s="26"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -1024,9 +1042,10 @@
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="26"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U15" s="7"/>
+      <c r="V15" s="26"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -1047,9 +1066,10 @@
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
-      <c r="U16" s="26"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16" s="7"/>
+      <c r="V16" s="26"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -1070,9 +1090,10 @@
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="26"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="7"/>
+      <c r="V17" s="26"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -1093,9 +1114,10 @@
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
-      <c r="U18" s="26"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U18" s="7"/>
+      <c r="V18" s="26"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
@@ -1116,9 +1138,10 @@
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
-      <c r="U19" s="26"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U19" s="7"/>
+      <c r="V19" s="26"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
@@ -1139,9 +1162,10 @@
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
-      <c r="U20" s="26"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U20" s="7"/>
+      <c r="V20" s="26"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
@@ -1162,9 +1186,10 @@
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="26"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="7"/>
+      <c r="V21" s="26"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
@@ -1185,9 +1210,10 @@
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
-      <c r="U22" s="26"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U22" s="7"/>
+      <c r="V22" s="26"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
@@ -1208,9 +1234,10 @@
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
-      <c r="U23" s="26"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U23" s="7"/>
+      <c r="V23" s="26"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
@@ -1231,9 +1258,10 @@
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
-      <c r="U24" s="26"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U24" s="7"/>
+      <c r="V24" s="26"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -1254,9 +1282,10 @@
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
-      <c r="U25" s="26"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="7"/>
+      <c r="V25" s="26"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1277,9 +1306,10 @@
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
-      <c r="U26" s="26"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U26" s="7"/>
+      <c r="V26" s="26"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
@@ -1300,9 +1330,10 @@
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
-      <c r="U27" s="26"/>
-    </row>
-    <row r="28" spans="1:21" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U27" s="7"/>
+      <c r="V27" s="26"/>
+    </row>
+    <row r="28" spans="1:22" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
         <v>22</v>
       </c>
@@ -1339,13 +1370,14 @@
         <f>SUM(S$4:S26)</f>
         <v>0</v>
       </c>
-      <c r="T28" s="33">
-        <f>SUM(T$4:T26)</f>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33">
+        <f>SUM(U$4:U26)</f>
         <v>0</v>
       </c>
-      <c r="U28" s="38"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="38"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="12"/>
       <c r="C29" s="8"/>
@@ -1366,11 +1398,12 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
-      <c r="U29" s="27"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A1:V1"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>